<commit_message>
Emplicacion y cambio de la db - Sesion 1
</commit_message>
<xml_diff>
--- a/planificacion proyecto Final.xlsx
+++ b/planificacion proyecto Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruralkeymaster\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ingsoft-dicama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{792CFB0E-5991-4ACB-8677-B288C0FA2BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268BF163-F349-48FF-86B5-9B9A03FCC3C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E0461C9-EB88-46E6-A804-4C1693C96CB7}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{6E0461C9-EB88-46E6-A804-4C1693C96CB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Reportes e Implementacion</t>
   </si>
   <si>
-    <t>Login de Empleado y Creacion de Usuarios.</t>
-  </si>
-  <si>
     <t>Base de Datos a Nivel de Tablas.</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Exportar a PDF, Exportar a Excel.</t>
+  </si>
+  <si>
+    <t>Login de Empleado y Creacion de Usuarios. --PENDIENTE l acreacion de usuarios</t>
   </si>
 </sst>
 </file>
@@ -284,14 +284,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -610,37 +610,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C099CA98-5A73-4F41-ACEE-47375A284956}">
   <dimension ref="C3:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="6"/>
+    <col min="1" max="1" width="3.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="7" style="6" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="27.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="102" style="6" customWidth="1"/>
-    <col min="9" max="9" width="83.85546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="94.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="79" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" style="6" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" style="6" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
     </row>
     <row r="4" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="7"/>
@@ -670,10 +671,10 @@
         <v>4</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
@@ -684,7 +685,7 @@
       <c r="C6" s="2">
         <v>44263</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -705,7 +706,7 @@
       <c r="C7" s="2">
         <v>44266</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
@@ -716,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -726,7 +727,7 @@
       <c r="C8" s="2">
         <v>44270</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -747,7 +748,7 @@
       <c r="C9" s="2">
         <v>44273</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
@@ -758,10 +759,10 @@
         <v>9</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -770,7 +771,7 @@
       <c r="C10" s="2">
         <v>44277</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="11">
         <v>3</v>
       </c>
       <c r="E10" s="3" t="s">
@@ -791,7 +792,7 @@
       <c r="C11" s="2">
         <v>44280</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
@@ -802,10 +803,10 @@
         <v>10</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -814,7 +815,7 @@
       <c r="C12" s="2">
         <v>44284</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="11">
         <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -835,7 +836,7 @@
       <c r="C13" s="2">
         <v>44287</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="3" t="s">
         <v>8</v>
       </c>
@@ -846,10 +847,10 @@
         <v>10</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -858,7 +859,7 @@
       <c r="C14" s="2">
         <v>44291</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="11">
         <v>5</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -879,7 +880,7 @@
       <c r="C15" s="2">
         <v>44294</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="3" t="s">
         <v>8</v>
       </c>
@@ -890,10 +891,10 @@
         <v>11</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -902,7 +903,7 @@
       <c r="C16" s="2">
         <v>44298</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>6</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -923,7 +924,7 @@
       <c r="C17" s="2">
         <v>44301</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="3" t="s">
         <v>8</v>
       </c>
@@ -934,10 +935,10 @@
         <v>11</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -946,7 +947,7 @@
       <c r="C18" s="2">
         <v>44305</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="11">
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
@@ -967,7 +968,7 @@
       <c r="C19" s="2">
         <v>44308</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="3" t="s">
         <v>8</v>
       </c>
@@ -978,10 +979,10 @@
         <v>12</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -990,7 +991,7 @@
       <c r="C20" s="2">
         <v>44312</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="11">
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
@@ -1011,7 +1012,7 @@
       <c r="C21" s="2">
         <v>44315</v>
       </c>
-      <c r="D21" s="11"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1022,7 +1023,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1032,7 +1033,7 @@
       <c r="C22" s="2">
         <v>44319</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="11">
         <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
@@ -1053,7 +1054,7 @@
       <c r="C23" s="2">
         <v>44322</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1064,10 +1065,10 @@
         <v>9</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1076,7 +1077,7 @@
       <c r="C24" s="2">
         <v>44326</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="11">
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
@@ -1097,7 +1098,7 @@
       <c r="C25" s="2">
         <v>44329</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1108,10 +1109,10 @@
         <v>10</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -1120,7 +1121,7 @@
       <c r="C26" s="2">
         <v>44333</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="11">
         <v>11</v>
       </c>
       <c r="E26" s="3" t="s">
@@ -1141,7 +1142,7 @@
       <c r="C27" s="2">
         <v>44336</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="3" t="s">
         <v>8</v>
       </c>
@@ -1152,10 +1153,10 @@
         <v>11</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
@@ -1164,7 +1165,7 @@
       <c r="C28" s="2">
         <v>44340</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="11">
         <v>12</v>
       </c>
       <c r="E28" s="3" t="s">
@@ -1185,7 +1186,7 @@
       <c r="C29" s="2">
         <v>44343</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="3" t="s">
         <v>8</v>
       </c>
@@ -1196,10 +1197,10 @@
         <v>13</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
@@ -1239,11 +1240,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="D24:D25"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D28:D29"/>
@@ -1252,6 +1248,11 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1259,15 +1260,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E6C08904C76F7D47929C9BCD2A83891D" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e08d2322c4f9540867bfba37c286d08a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fd3b4c0a-8b7f-42a3-8d2a-31cd68cffff8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfd3880fed17414b4cb52f079abf3c22" ns3:_="">
     <xsd:import namespace="fd3b4c0a-8b7f-42a3-8d2a-31cd68cffff8"/>
@@ -1413,6 +1405,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1420,14 +1421,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE1AE11-30B5-49EE-94A7-194A868690A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EC0F1B4-A204-48B0-8DBF-DF7C6DE1200F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1441,6 +1434,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CE1AE11-30B5-49EE-94A7-194A868690A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>